<commit_message>
Correct old instrument names and spelling
</commit_message>
<xml_diff>
--- a/product-definitions/spreadsheet/_instrument_vocabs.xlsx
+++ b/product-definitions/spreadsheet/_instrument_vocabs.xlsx
@@ -791,7 +791,7 @@
     <t>Ultramet 6E</t>
   </si>
   <si>
-    <t>wao-siemens-oxzilla</t>
+    <t>wao-CO2</t>
   </si>
   <si>
     <t>ncas-co2-1</t>
@@ -1652,6 +1652,9 @@
     <t>Oxzilla II</t>
   </si>
   <si>
+    <t>wao-O2</t>
+  </si>
+  <si>
     <t>ncas-o2-1</t>
   </si>
   <si>
@@ -2041,9 +2044,6 @@
   </si>
   <si>
     <t>ncas-rapidsonde-1</t>
-  </si>
-  <si>
-    <t>Machester</t>
   </si>
   <si>
     <t>NCAS Windsond Sounding Station unit 1</t>
@@ -2377,7 +2377,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2437,6 +2437,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
@@ -32373,7 +32376,7 @@
         <v>255</v>
       </c>
       <c r="D38" s="10"/>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="20" t="s">
         <v>256</v>
       </c>
       <c r="F38" s="6" t="s">
@@ -33086,7 +33089,7 @@
       <c r="B57" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="21" t="s">
         <v>321</v>
       </c>
       <c r="D57" s="10"/>
@@ -33202,7 +33205,7 @@
       <c r="C60" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D60" s="22" t="s">
         <v>338</v>
       </c>
       <c r="E60" s="14"/>
@@ -33241,7 +33244,7 @@
       <c r="C61" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D61" s="22" t="s">
         <v>343</v>
       </c>
       <c r="E61" s="14"/>
@@ -33358,7 +33361,7 @@
       <c r="C64" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="D64" s="21" t="s">
+      <c r="D64" s="22" t="s">
         <v>359</v>
       </c>
       <c r="E64" s="14"/>
@@ -33397,7 +33400,7 @@
       <c r="C65" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="D65" s="21" t="s">
+      <c r="D65" s="22" t="s">
         <v>364</v>
       </c>
       <c r="E65" s="14"/>
@@ -33621,7 +33624,7 @@
       <c r="C71" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="D71" s="22">
+      <c r="D71" s="23">
         <v>30123.0</v>
       </c>
       <c r="E71" s="14"/>
@@ -33697,7 +33700,7 @@
       <c r="C73" s="13" t="s">
         <v>401</v>
       </c>
-      <c r="D73" s="23" t="s">
+      <c r="D73" s="24" t="s">
         <v>402</v>
       </c>
       <c r="E73" s="14"/>
@@ -33736,7 +33739,7 @@
       <c r="C74" s="13" t="s">
         <v>401</v>
       </c>
-      <c r="D74" s="21" t="s">
+      <c r="D74" s="22" t="s">
         <v>406</v>
       </c>
       <c r="E74" s="14"/>
@@ -34461,7 +34464,7 @@
       <c r="C93" s="13" t="s">
         <v>495</v>
       </c>
-      <c r="D93" s="24" t="s">
+      <c r="D93" s="25" t="s">
         <v>496</v>
       </c>
       <c r="E93" s="15" t="s">
@@ -34645,7 +34648,7 @@
       <c r="B98" s="8" t="s">
         <v>509</v>
       </c>
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="21" t="s">
         <v>514</v>
       </c>
       <c r="D98" s="10"/>
@@ -34795,18 +34798,18 @@
       <c r="B102" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="C102" s="25" t="s">
+      <c r="C102" s="26" t="s">
         <v>527</v>
       </c>
       <c r="D102" s="10"/>
-      <c r="E102" s="6" t="s">
-        <v>256</v>
+      <c r="E102" s="20" t="s">
+        <v>528</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="H102" s="6" t="s">
         <v>18</v>
@@ -34821,7 +34824,7 @@
         <v>33</v>
       </c>
       <c r="L102" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M102" s="6" t="s">
         <v>80</v>
@@ -34832,17 +34835,17 @@
         <v>41</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C103" s="6">
         <v>202.0</v>
       </c>
       <c r="D103" s="10"/>
       <c r="E103" s="6" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>44</v>
@@ -34860,7 +34863,7 @@
         <v>33</v>
       </c>
       <c r="L103" s="6" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="M103" s="7" t="s">
         <v>100</v>
@@ -34871,17 +34874,17 @@
         <v>41</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C104" s="6">
         <v>205.0</v>
       </c>
       <c r="D104" s="10"/>
       <c r="E104" s="6" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>44</v>
@@ -34899,7 +34902,7 @@
         <v>33</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M104" s="7" t="s">
         <v>100</v>
@@ -34913,14 +34916,14 @@
         <v>36</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D105" s="10"/>
       <c r="E105" s="6" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>44</v>
@@ -34938,7 +34941,7 @@
         <v>33</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="M105" s="7" t="s">
         <v>100</v>
@@ -34956,10 +34959,10 @@
       </c>
       <c r="D106" s="10"/>
       <c r="E106" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>44</v>
@@ -34977,7 +34980,7 @@
         <v>33</v>
       </c>
       <c r="L106" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="M106" s="7" t="s">
         <v>80</v>
@@ -34996,7 +34999,7 @@
       <c r="D107" s="10"/>
       <c r="E107" s="4"/>
       <c r="F107" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>44</v>
@@ -35014,7 +35017,7 @@
         <v>33</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M107" s="7" t="s">
         <v>80</v>
@@ -35032,10 +35035,10 @@
       </c>
       <c r="D108" s="10"/>
       <c r="E108" s="6" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>44</v>
@@ -35053,7 +35056,7 @@
         <v>33</v>
       </c>
       <c r="L108" s="6" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="M108" s="7" t="s">
         <v>100</v>
@@ -35061,7 +35064,7 @@
     </row>
     <row r="109">
       <c r="A109" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>347</v>
@@ -35072,10 +35075,10 @@
       <c r="D109" s="10"/>
       <c r="E109" s="4"/>
       <c r="F109" s="6" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="H109" s="8" t="s">
         <v>76</v>
@@ -35090,31 +35093,31 @@
         <v>33</v>
       </c>
       <c r="L109" s="6" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="M109" s="7" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="8" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E110" s="10"/>
       <c r="F110" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="H110" s="8" t="s">
         <v>113</v>
@@ -35126,10 +35129,10 @@
         <v>114</v>
       </c>
       <c r="K110" s="8" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="L110" s="8" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="M110" s="8" t="s">
         <v>80</v>
@@ -35137,18 +35140,18 @@
     </row>
     <row r="111">
       <c r="A111" s="8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>181</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D111" s="10"/>
       <c r="E111" s="10"/>
       <c r="F111" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>17</v>
@@ -35166,7 +35169,7 @@
         <v>21</v>
       </c>
       <c r="L111" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="M111" s="8" t="s">
         <v>80</v>
@@ -35174,20 +35177,20 @@
     </row>
     <row r="112">
       <c r="A112" s="6" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>347</v>
       </c>
       <c r="D112" s="10"/>
       <c r="E112" s="6" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>305</v>
@@ -35199,13 +35202,13 @@
         <v>19</v>
       </c>
       <c r="J112" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="K112" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="M112" s="7" t="s">
         <v>80</v>
@@ -35213,17 +35216,17 @@
     </row>
     <row r="113">
       <c r="A113" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
       <c r="D113" s="10"/>
       <c r="E113" s="10"/>
       <c r="F113" s="8" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H113" s="8" t="s">
         <v>113</v>
@@ -35232,13 +35235,13 @@
         <v>107</v>
       </c>
       <c r="J113" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K113" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="K113" s="8" t="s">
-        <v>574</v>
-      </c>
       <c r="L113" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="M113" s="8" t="s">
         <v>80</v>
@@ -35246,17 +35249,17 @@
     </row>
     <row r="114">
       <c r="A114" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
       <c r="D114" s="10"/>
       <c r="E114" s="10"/>
       <c r="F114" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H114" s="8" t="s">
         <v>113</v>
@@ -35265,13 +35268,13 @@
         <v>107</v>
       </c>
       <c r="J114" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K114" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="K114" s="8" t="s">
-        <v>574</v>
-      </c>
       <c r="L114" s="8" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="M114" s="8" t="s">
         <v>80</v>
@@ -35279,17 +35282,17 @@
     </row>
     <row r="115">
       <c r="A115" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="8" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H115" s="8" t="s">
         <v>113</v>
@@ -35298,13 +35301,13 @@
         <v>107</v>
       </c>
       <c r="J115" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K115" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="K115" s="8" t="s">
-        <v>574</v>
-      </c>
       <c r="L115" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="M115" s="8" t="s">
         <v>80</v>
@@ -35312,21 +35315,21 @@
     </row>
     <row r="116">
       <c r="A116" s="6" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>64</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D116" s="10"/>
       <c r="E116" s="4"/>
       <c r="F116" s="6" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H116" s="6" t="s">
         <v>76</v>
@@ -35335,13 +35338,13 @@
         <v>107</v>
       </c>
       <c r="J116" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="K116" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="K116" s="6" t="s">
-        <v>574</v>
-      </c>
       <c r="L116" s="6" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="M116" s="6" t="s">
         <v>100</v>
@@ -35349,23 +35352,23 @@
     </row>
     <row r="117">
       <c r="A117" s="6" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D117" s="10"/>
       <c r="E117" s="6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H117" s="6" t="s">
         <v>76</v>
@@ -35377,10 +35380,10 @@
         <v>486</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="M117" s="6" t="s">
         <v>100</v>
@@ -35388,7 +35391,7 @@
     </row>
     <row r="118">
       <c r="A118" s="8" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>347</v>
@@ -35399,10 +35402,10 @@
       <c r="D118" s="10"/>
       <c r="E118" s="10"/>
       <c r="F118" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="H118" s="8" t="s">
         <v>106</v>
@@ -35414,10 +35417,10 @@
         <v>108</v>
       </c>
       <c r="K118" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="L118" s="8" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="M118" s="8" t="s">
         <v>80</v>
@@ -35425,23 +35428,23 @@
     </row>
     <row r="119">
       <c r="A119" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D119" s="10"/>
       <c r="E119" s="6" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="H119" s="6" t="s">
         <v>76</v>
@@ -35456,7 +35459,7 @@
         <v>68</v>
       </c>
       <c r="L119" s="6" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="M119" s="6" t="s">
         <v>100</v>
@@ -35464,23 +35467,23 @@
     </row>
     <row r="120">
       <c r="A120" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>181</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D120" s="10"/>
       <c r="E120" s="6" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G120" s="11" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H120" s="6" t="s">
         <v>76</v>
@@ -35495,7 +35498,7 @@
         <v>68</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="M120" s="6" t="s">
         <v>100</v>
@@ -35503,25 +35506,25 @@
     </row>
     <row r="121">
       <c r="A121" s="13" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B121" s="13" t="s">
         <v>181</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>604</v>
-      </c>
-      <c r="D121" s="26" t="s">
-        <v>610</v>
+        <v>605</v>
+      </c>
+      <c r="D121" s="27" t="s">
+        <v>611</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F121" s="13" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G121" s="15" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H121" s="13" t="s">
         <v>76</v>
@@ -35536,7 +35539,7 @@
         <v>68</v>
       </c>
       <c r="L121" s="13" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="M121" s="13" t="s">
         <v>100</v>
@@ -35544,20 +35547,20 @@
     </row>
     <row r="122">
       <c r="A122" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>616</v>
-      </c>
-      <c r="D122" s="27" t="s">
         <v>617</v>
+      </c>
+      <c r="D122" s="28" t="s">
+        <v>618</v>
       </c>
       <c r="E122" s="10"/>
       <c r="F122" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>357</v>
@@ -35575,7 +35578,7 @@
         <v>357</v>
       </c>
       <c r="L122" s="8" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="M122" s="8" t="s">
         <v>80</v>
@@ -35583,20 +35586,20 @@
     </row>
     <row r="123">
       <c r="A123" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D123" s="8">
         <v>120894.0</v>
       </c>
       <c r="E123" s="10"/>
       <c r="F123" s="8" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>357</v>
@@ -35614,7 +35617,7 @@
         <v>357</v>
       </c>
       <c r="L123" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="M123" s="8" t="s">
         <v>80</v>
@@ -35622,20 +35625,20 @@
     </row>
     <row r="124">
       <c r="A124" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D124" s="8">
         <v>10539.0</v>
       </c>
       <c r="E124" s="10"/>
       <c r="F124" s="8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="G124" s="11" t="s">
         <v>357</v>
@@ -35653,7 +35656,7 @@
         <v>357</v>
       </c>
       <c r="L124" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="M124" s="8" t="s">
         <v>80</v>
@@ -35661,20 +35664,20 @@
     </row>
     <row r="125">
       <c r="A125" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D125" s="8">
         <v>121016.0</v>
       </c>
       <c r="E125" s="10"/>
       <c r="F125" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="G125" s="11" t="s">
         <v>357</v>
@@ -35692,7 +35695,7 @@
         <v>357</v>
       </c>
       <c r="L125" s="8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="M125" s="8" t="s">
         <v>80</v>
@@ -35700,7 +35703,7 @@
     </row>
     <row r="126">
       <c r="A126" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>347</v>
@@ -35709,11 +35712,11 @@
         <v>347</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="E126" s="10"/>
       <c r="F126" s="8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G126" s="11" t="s">
         <v>331</v>
@@ -35731,7 +35734,7 @@
         <v>331</v>
       </c>
       <c r="L126" s="8" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="M126" s="8" t="s">
         <v>80</v>
@@ -35739,7 +35742,7 @@
     </row>
     <row r="127">
       <c r="A127" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B127" s="8" t="s">
         <v>347</v>
@@ -35748,11 +35751,11 @@
         <v>347</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E127" s="10"/>
       <c r="F127" s="8" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="G127" s="11" t="s">
         <v>331</v>
@@ -35770,7 +35773,7 @@
         <v>331</v>
       </c>
       <c r="L127" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="M127" s="8" t="s">
         <v>80</v>
@@ -35778,7 +35781,7 @@
     </row>
     <row r="128">
       <c r="A128" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>347</v>
@@ -35787,11 +35790,11 @@
         <v>347</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E128" s="10"/>
       <c r="F128" s="8" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="G128" s="11" t="s">
         <v>331</v>
@@ -35809,7 +35812,7 @@
         <v>331</v>
       </c>
       <c r="L128" s="8" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="M128" s="8" t="s">
         <v>80</v>
@@ -35817,20 +35820,20 @@
     </row>
     <row r="129">
       <c r="A129" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D129" s="8">
         <v>367792.0</v>
       </c>
       <c r="E129" s="10"/>
       <c r="F129" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>331</v>
@@ -35848,7 +35851,7 @@
         <v>331</v>
       </c>
       <c r="L129" s="8" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M129" s="8" t="s">
         <v>80</v>
@@ -35856,18 +35859,18 @@
     </row>
     <row r="130">
       <c r="A130" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C130" s="10"/>
-      <c r="D130" s="28" t="s">
-        <v>644</v>
+      <c r="D130" s="29" t="s">
+        <v>645</v>
       </c>
       <c r="E130" s="10"/>
       <c r="F130" s="8" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="G130" s="11" t="s">
         <v>331</v>
@@ -35885,7 +35888,7 @@
         <v>331</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="M130" s="8" t="s">
         <v>80</v>
@@ -35893,18 +35896,18 @@
     </row>
     <row r="131">
       <c r="A131" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C131" s="10"/>
       <c r="D131" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E131" s="10"/>
       <c r="F131" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="G131" s="11" t="s">
         <v>331</v>
@@ -35922,7 +35925,7 @@
         <v>331</v>
       </c>
       <c r="L131" s="8" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M131" s="8" t="s">
         <v>80</v>
@@ -35930,18 +35933,18 @@
     </row>
     <row r="132">
       <c r="A132" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>347</v>
       </c>
       <c r="C132" s="10"/>
       <c r="D132" s="8" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E132" s="10"/>
       <c r="F132" s="8" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="G132" s="11" t="s">
         <v>331</v>
@@ -35959,7 +35962,7 @@
         <v>331</v>
       </c>
       <c r="L132" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="M132" s="8" t="s">
         <v>80</v>
@@ -35967,27 +35970,27 @@
     </row>
     <row r="133">
       <c r="A133" s="6" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D133" s="10"/>
       <c r="E133" s="4"/>
       <c r="F133" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H133" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I133" s="6" t="s">
-        <v>658</v>
+      <c r="I133" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="J133" s="8" t="s">
         <v>424</v>
@@ -36007,12 +36010,12 @@
         <v>660</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>656</v>
-      </c>
-      <c r="D134" s="29">
+        <v>657</v>
+      </c>
+      <c r="D134" s="30">
         <v>43867.0</v>
       </c>
       <c r="E134" s="14"/>
@@ -36020,7 +36023,7 @@
         <v>661</v>
       </c>
       <c r="G134" s="15" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H134" s="13" t="s">
         <v>76</v>
@@ -36314,7 +36317,7 @@
       <c r="C142" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="D142" s="26" t="s">
+      <c r="D142" s="27" t="s">
         <v>685</v>
       </c>
       <c r="E142" s="13" t="s">
@@ -36355,7 +36358,7 @@
       <c r="C143" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="D143" s="26" t="s">
+      <c r="D143" s="27" t="s">
         <v>690</v>
       </c>
       <c r="E143" s="13" t="s">
@@ -36396,7 +36399,7 @@
       <c r="C144" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="D144" s="26" t="s">
+      <c r="D144" s="27" t="s">
         <v>694</v>
       </c>
       <c r="E144" s="13" t="s">
@@ -36626,7 +36629,7 @@
       <c r="C150" s="13" t="s">
         <v>720</v>
       </c>
-      <c r="D150" s="22">
+      <c r="D150" s="23">
         <v>155.0</v>
       </c>
       <c r="E150" s="14"/>
@@ -36734,125 +36737,125 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="30" t="s">
+      <c r="A153" s="31" t="s">
         <v>731</v>
       </c>
-      <c r="B153" s="30" t="s">
+      <c r="B153" s="31" t="s">
         <v>732</v>
       </c>
-      <c r="C153" s="30" t="s">
+      <c r="C153" s="31" t="s">
         <v>733</v>
       </c>
-      <c r="D153" s="30">
+      <c r="D153" s="31">
         <v>5.83053001031E11</v>
       </c>
-      <c r="E153" s="30" t="s">
+      <c r="E153" s="31" t="s">
         <v>734</v>
       </c>
-      <c r="F153" s="30" t="s">
+      <c r="F153" s="31" t="s">
         <v>735</v>
       </c>
-      <c r="G153" s="30" t="s">
+      <c r="G153" s="31" t="s">
         <v>736</v>
       </c>
-      <c r="H153" s="30" t="s">
+      <c r="H153" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="I153" s="30" t="s">
+      <c r="I153" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="J153" s="30" t="s">
+      <c r="J153" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="K153" s="30" t="s">
+      <c r="K153" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="L153" s="30" t="s">
+      <c r="L153" s="31" t="s">
         <v>737</v>
       </c>
-      <c r="M153" s="30" t="s">
+      <c r="M153" s="31" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="30" t="s">
+      <c r="A154" s="31" t="s">
         <v>731</v>
       </c>
-      <c r="B154" s="30" t="s">
+      <c r="B154" s="31" t="s">
         <v>732</v>
       </c>
-      <c r="C154" s="30" t="s">
+      <c r="C154" s="31" t="s">
         <v>733</v>
       </c>
-      <c r="D154" s="30">
+      <c r="D154" s="31">
         <v>5.83053001033E11</v>
       </c>
-      <c r="E154" s="30" t="s">
+      <c r="E154" s="31" t="s">
         <v>734</v>
       </c>
-      <c r="F154" s="30" t="s">
+      <c r="F154" s="31" t="s">
         <v>738</v>
       </c>
-      <c r="G154" s="30" t="s">
+      <c r="G154" s="31" t="s">
         <v>736</v>
       </c>
-      <c r="H154" s="30" t="s">
+      <c r="H154" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="I154" s="30" t="s">
+      <c r="I154" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="J154" s="30" t="s">
+      <c r="J154" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="K154" s="30" t="s">
+      <c r="K154" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="L154" s="30" t="s">
+      <c r="L154" s="31" t="s">
         <v>739</v>
       </c>
-      <c r="M154" s="30" t="s">
+      <c r="M154" s="31" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="30" t="s">
+      <c r="A155" s="31" t="s">
         <v>740</v>
       </c>
-      <c r="B155" s="30" t="s">
+      <c r="B155" s="31" t="s">
         <v>741</v>
       </c>
-      <c r="C155" s="30" t="s">
+      <c r="C155" s="31" t="s">
         <v>742</v>
       </c>
-      <c r="D155" s="30">
+      <c r="D155" s="31">
         <v>2208392.0</v>
       </c>
-      <c r="E155" s="30" t="s">
+      <c r="E155" s="31" t="s">
         <v>734</v>
       </c>
-      <c r="F155" s="30" t="s">
+      <c r="F155" s="31" t="s">
         <v>743</v>
       </c>
-      <c r="G155" s="30" t="s">
-        <v>574</v>
-      </c>
-      <c r="H155" s="30" t="s">
+      <c r="G155" s="31" t="s">
+        <v>575</v>
+      </c>
+      <c r="H155" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="I155" s="30" t="s">
+      <c r="I155" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="J155" s="30" t="s">
+      <c r="J155" s="31" t="s">
         <v>486</v>
       </c>
-      <c r="K155" s="30" t="s">
-        <v>574</v>
-      </c>
-      <c r="L155" s="30" t="s">
+      <c r="K155" s="31" t="s">
+        <v>575</v>
+      </c>
+      <c r="L155" s="31" t="s">
         <v>744</v>
       </c>
-      <c r="M155" s="30" t="s">
+      <c r="M155" s="31" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>